<commit_message>
user online & indexing
</commit_message>
<xml_diff>
--- a/public/be_tempImportExam.xlsx
+++ b/public/be_tempImportExam.xlsx
@@ -15,28 +15,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">TEMPLATE UJIAN URAIAN
-</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>SOAL</t>
-  </si>
-  <si>
-    <t>Ayam apa yang ayam kampung hayo ayam ?</t>
-  </si>
-  <si>
-    <t>Kapal kapal apa yang api ?</t>
-  </si>
-  <si>
-    <t>Kenapa bisa kenapa ?</t>
-  </si>
-  <si>
-    <t>Siapa yang bertanya bisa kenapa ?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+  <si>
+    <t>KODE</t>
+  </si>
+  <si>
+    <t>JENIS</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>JAWABAN</t>
+  </si>
+  <si>
+    <t>9fc8747327</t>
+  </si>
+  <si>
+    <t>Soal</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>ea4c51af01</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>0a8e95c43c</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>be_b7671299-bfdd-4dc8-b818-0984e3fb54fe.jpeg</t>
+  </si>
+  <si>
+    <t>be_70b1b0dd-6954-4b67-8b8f-182b17f7581c.jpeg</t>
+  </si>
+  <si>
+    <t>be_dfab805d-3d29-4b8e-8351-789b138a66da.jpeg</t>
+  </si>
+  <si>
+    <t>be_c10303fe-28f9-4b1c-b33d-1d86f513b3d1.png</t>
   </si>
 </sst>
 </file>
@@ -63,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -71,32 +106,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -104,6 +120,159 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1228725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 2" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="1638300" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1143000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 4" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="1343025" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2343150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 6" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="1790700" cy="2257425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 8" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0">
+          <a:ext cx="828675" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,83 +565,249 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="28.85546875" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" customHeight="1" ht="99">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" customHeight="1" ht="91.5">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" customHeight="1" ht="28.5">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customHeight="1" ht="184.5">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1"/>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -485,6 +820,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>